<commit_message>
add sample to saple inbound mappings
</commit_message>
<xml_diff>
--- a/resources/samples/SampleMappings_13.xlsx
+++ b/resources/samples/SampleMappings_13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ck/work/git/cumulocity-dynamic-mapper/resources/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AE369EB-E584-4502-BECE-150DB477B13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F22DCA35-1029-4893-A17B-8A27C6682C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10040" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{B5E387B2-3E90-884E-B546-D827ECD68714}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$G$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$G$29</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="147">
   <si>
     <t>Sample Mapping #</t>
   </si>
@@ -647,7 +647,7 @@
   </si>
   <si>
     <t xml:space="preserve"> 
-Use test client: cumulocity-dynamic-mapper/mqtt-mapping-extension/src/test/java/dynamic/mapping/ProtobufMqttClient.java
+Use test client: cumulocity-dynamic-mapper/dynamic-mapping-extension/src/test/java/dynamic/mapping/ProtobufMqttClient.java
 to create a new event for bus "berlin_01"</t>
   </si>
   <si>
@@ -793,8 +793,8 @@
 mapppingType: Processor Extension Source
 check: Use external id
 sub:
-Events for mqtt-mapping-extension: CustomMeasurement
-Extension for PROCESSOR_EXTENSION: mqtt-mapping-externsion
+Extension for PROCESSOR_EXTENSION_SOURCE: dynamic-mapping-externsion
+Events for dynamic-mapping-extension: CustomMeasurement
 Defined in cumulocity-dynamic-mapper/dynamic-mapping-extension/src/main/java/dynamic/mapping/processor/extension/external/ProcessorExtensionCustomMeasurement.java
 </t>
   </si>
@@ -918,6 +918,36 @@
   </si>
   <si>
     <t>Map the structure under meas as fragments in the measurements. The number of keys in meas can vary and must therefore be generated dynamically.</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>XTENSION_SOURCE_TARGET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mappingTopic:       extension/source_target
+mappingTopicSample: extension/source_target
+check: Use external id
+Extensions for Processor Extension Source Target:
+select 
+Events for:
+select
+Defined in cumulocity-dynamic-mapper/dynamic-mapping-extension/src/main/java/dynamic/mapping/processor/extension/external/ProcessorExtensionCustomAlarm.java
+</t>
+  </si>
+  <si>
+    <t>{
+    "alarmType": "MAJOR",
+    "message": "This is an alamr for the extension!",
+    "type": "c8y_ExtensionAlarm",
+    "externalId": "berlin_01",
+    "time": "2024-06-18T13:20:45.000Z"
+}</t>
+  </si>
+  <si>
+    <t>the extraction and the substitution in the tagetPayload are implemented in java, see. ProcessorExtensionCustomAlarm.java.
+This is useful if the processing of the source payload can't be achieved in JSONata and the building of the tragetP payload (Cumulocity) cant be achieved by standard substitutions.</t>
   </si>
   <si>
     <t>JSON
@@ -1499,10 +1529,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="142" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2045,7 +2075,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="206.25" customHeight="1">
+    <row r="24" spans="1:7" ht="177" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>122</v>
       </c>
@@ -2068,24 +2098,24 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="163.5">
-      <c r="A25" s="9">
-        <v>51</v>
-      </c>
-      <c r="B25" s="10" t="s">
+    <row r="25" spans="1:7" ht="206.25" customHeight="1">
+      <c r="A25" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="B25" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>131</v>
@@ -2093,75 +2123,98 @@
     </row>
     <row r="26" spans="1:7" ht="163.5">
       <c r="A26" s="9">
+        <v>51</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="163.5">
+      <c r="A27" s="9">
         <v>52</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B27" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="174.75">
-      <c r="A27" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="174.75">
       <c r="A28" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="F30" s="6"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="174.75">
+      <c r="A29" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="F31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
@@ -2170,7 +2223,7 @@
     <oddFooter>Page &amp;P&amp;R&amp;F</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="24" max="6" man="1"/>
+    <brk id="25" max="6" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add connectors in as navigation nodes
</commit_message>
<xml_diff>
--- a/resources/samples/SampleMappings_13.xlsx
+++ b/resources/samples/SampleMappings_13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ck/work/git/cumulocity-dynamic-mapper/resources/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B0A6AEB-2CDF-488B-98CE-5058BFDBB572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BEFF138-6A67-4F9F-943E-0430655D707D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10040" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{B5E387B2-3E90-884E-B546-D827ECD68714}"/>
   </bookViews>
@@ -612,7 +612,7 @@
     <t>15</t>
   </si>
   <si>
-    <t>PROCESSOR_EXTENSION_SOURCE</t>
+    <t>EXTENSION_SOURCE</t>
   </si>
   <si>
     <t xml:space="preserve">mappingTopic:        protobuf/event
@@ -923,7 +923,7 @@
     <t>24</t>
   </si>
   <si>
-    <t>XTENSION_SOURCE_TARGET</t>
+    <t>EXTENSION_SOURCE_TARGET</t>
   </si>
   <si>
     <t xml:space="preserve">mappingTopic:       extension/source_target
@@ -981,7 +981,7 @@
       </rPr>
       <t xml:space="preserve"> 
 sub:
-1.	[ bus_id -&gt; _IDENTITY_.c8ySourceId ]
+1.	[ bus_c8ySourceId -&gt; _IDENTITY_.c8ySourceId ]
 2.	[ msg_type -&gt; type ]
 3.	[ tx -&gt; text ]</t>
     </r>
@@ -1212,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1273,6 +1273,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1593,15 +1596,15 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="142" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" style="11"/>
-    <col min="2" max="2" width="18.875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="51.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="11" customWidth="1"/>
+    <col min="3" max="3" width="54" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" style="15"/>
     <col min="5" max="5" width="46" style="1" customWidth="1"/>
     <col min="6" max="6" width="44" style="1" customWidth="1"/>
@@ -1612,7 +1615,7 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">

</xml_diff>